<commit_message>
checks for req auth 5 on admin page
</commit_message>
<xml_diff>
--- a/teknisk_dokumentasjon.xlsx
+++ b/teknisk_dokumentasjon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simen\git_stuff\barcode-scanning-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F21FFBE-7865-4753-B3FF-849489D64621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45166D4D-6221-4CDC-BF6E-015036DE7D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B4F523E-6B92-466C-90AA-6FAA4E138F36}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>hostname:</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>simen pass:</t>
+  </si>
+  <si>
+    <t>ip:</t>
+  </si>
+  <si>
+    <t>10.10.69.69</t>
   </si>
 </sst>
 </file>
@@ -408,19 +414,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340C0E2E-4D60-4DCF-9289-C932750200FD}">
-  <dimension ref="C4:D8"/>
+  <dimension ref="C4:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -428,7 +434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -436,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -444,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -452,12 +458,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added .. to setup.js
</commit_message>
<xml_diff>
--- a/teknisk_dokumentasjon.xlsx
+++ b/teknisk_dokumentasjon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simen\git_stuff\barcode-scanning-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45166D4D-6221-4CDC-BF6E-015036DE7D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB894E9D-71F2-4D7B-AD89-4D596948F9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B4F523E-6B92-466C-90AA-6FAA4E138F36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B4F523E-6B92-466C-90AA-6FAA4E138F36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>hostname:</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>10.10.69.69</t>
+  </si>
+  <si>
+    <t>website:</t>
+  </si>
+  <si>
+    <t>admin username:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin password: </t>
+  </si>
+  <si>
+    <t>user username:</t>
+  </si>
+  <si>
+    <t>simen2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user password: </t>
   </si>
 </sst>
 </file>
@@ -414,43 +432,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340C0E2E-4D60-4DCF-9289-C932750200FD}">
-  <dimension ref="C4:D9"/>
+  <dimension ref="C4:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -458,20 +493,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>